<commit_message>
update all required variable to be included
</commit_message>
<xml_diff>
--- a/company_data/Company 12 Data.xlsx
+++ b/company_data/Company 12 Data.xlsx
@@ -9,14 +9,14 @@
   <sheets>
     <sheet r:id="rId1" sheetId="1" name="main_variables"/>
     <sheet r:id="rId2" sheetId="2" name="net_cash_flow"/>
-    <sheet r:id="rId3" sheetId="3" name="Copy of Compare P&amp;amp;amp;L Report_Mode"/>
+    <sheet r:id="rId3" sheetId="3" name="Copy of Compare P&amp;amp;amp;amp;amp;amp;L Report_Mode"/>
   </sheets>
   <calcPr fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="94">
   <si>
     <t>CS 12.1</t>
   </si>
@@ -290,6 +290,15 @@
   <si>
     <t>Net Sales Growth</t>
   </si>
+  <si>
+    <t>Relative Variation of Net Sales</t>
+  </si>
+  <si>
+    <t>Number of Active Patients</t>
+  </si>
+  <si>
+    <t>Relative Variation of Patient Spending</t>
+  </si>
 </sst>
 </file>
 
@@ -298,7 +307,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="#,##0%"/>
   </numFmts>
-  <fonts count="15" x14ac:knownFonts="1">
+  <fonts count="14" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -308,7 +317,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
@@ -353,12 +362,6 @@
     </font>
     <font>
       <b/>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
@@ -537,7 +540,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="94">
+  <cellXfs count="92">
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="general"/>
@@ -662,16 +665,16 @@
     <xf xfId="0" numFmtId="164" applyNumberFormat="1" borderId="7" applyBorder="1" fontId="4" applyFont="1" fillId="3" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf xfId="0" numFmtId="164" applyNumberFormat="1" borderId="2" applyBorder="1" fontId="9" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
+    <xf xfId="0" numFmtId="164" applyNumberFormat="1" borderId="2" applyBorder="1" fontId="1" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="4" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="10" applyFont="1" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="9" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf xfId="0" numFmtId="164" applyNumberFormat="1" borderId="2" applyBorder="1" fontId="11" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
+    <xf xfId="0" numFmtId="164" applyNumberFormat="1" borderId="2" applyBorder="1" fontId="10" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="3" applyBorder="1" fontId="4" applyFont="1" fillId="0" applyAlignment="1">
@@ -683,7 +686,7 @@
     <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="4" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf xfId="0" numFmtId="164" applyNumberFormat="1" borderId="6" applyBorder="1" fontId="9" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
+    <xf xfId="0" numFmtId="164" applyNumberFormat="1" borderId="6" applyBorder="1" fontId="1" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="4" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
@@ -695,13 +698,13 @@
     <xf xfId="0" numFmtId="164" applyNumberFormat="1" borderId="5" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="12" applyFont="1" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="11" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="2" applyBorder="1" fontId="2" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="2" applyBorder="1" fontId="13" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="2" applyBorder="1" fontId="12" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
@@ -737,19 +740,16 @@
     <xf xfId="0" numFmtId="164" applyNumberFormat="1" borderId="2" applyBorder="1" fontId="4" applyFont="1" fillId="3" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf xfId="0" numFmtId="164" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="9" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf xfId="0" numFmtId="0" borderId="8" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="2" applyBorder="1" fontId="9" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="2" applyBorder="1" fontId="1" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf xfId="0" numFmtId="164" applyNumberFormat="1" borderId="2" applyBorder="1" fontId="14" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
+    <xf xfId="0" numFmtId="164" applyNumberFormat="1" borderId="2" applyBorder="1" fontId="13" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="2" applyBorder="1" fontId="11" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="2" applyBorder="1" fontId="10" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="2" applyBorder="1" fontId="8" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
@@ -761,29 +761,26 @@
     <xf xfId="0" numFmtId="164" applyNumberFormat="1" borderId="2" applyBorder="1" fontId="2" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="2" applyBorder="1" fontId="11" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="2" applyBorder="1" fontId="10" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="2" applyBorder="1" fontId="9" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="2" applyBorder="1" fontId="1" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="general"/>
     </xf>
     <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general"/>
+      <alignment horizontal="right"/>
     </xf>
     <xf xfId="0" numFmtId="164" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="right"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf xfId="0" numFmtId="164" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general"/>
+      <alignment horizontal="right"/>
     </xf>
     <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -812,7 +809,7 @@
     <xf xfId="0" numFmtId="1" applyNumberFormat="1" borderId="2" applyBorder="1" fontId="2" applyFont="1" fillId="5" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="9" applyFont="1" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
@@ -1120,19 +1117,19 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:D15"/>
+  <dimension ref="A1:D18"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="1"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" style="93" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="93" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="93" width="37.005" customWidth="1" bestFit="1"/>
-    <col min="4" max="4" style="83" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" style="91" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="91" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="3" max="3" style="91" width="37.005" customWidth="1" bestFit="1"/>
+    <col min="4" max="4" style="81" width="13.576428571428572" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
-    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="19.5">
       <c r="A1" s="43" t="s">
         <v>75</v>
       </c>
@@ -1142,204 +1139,246 @@
       <c r="C1" s="43" t="s">
         <v>77</v>
       </c>
-      <c r="D1" s="89" t="s">
+      <c r="D1" s="87" t="s">
         <v>78</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="18.75">
-      <c r="A2" s="90" t="s">
+    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="19.5">
+      <c r="A2" s="88" t="s">
         <v>79</v>
       </c>
-      <c r="B2" s="90" t="s">
+      <c r="B2" s="88" t="s">
         <v>19</v>
       </c>
-      <c r="C2" s="90" t="s">
+      <c r="C2" s="88" t="s">
         <v>80</v>
       </c>
-      <c r="D2" s="87">
+      <c r="D2" s="85">
         <v>1486403.39</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="18.75">
-      <c r="A3" s="90" t="s">
+    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="19.5">
+      <c r="A3" s="88" t="s">
         <v>79</v>
       </c>
-      <c r="B3" s="90" t="s">
+      <c r="B3" s="88" t="s">
         <v>19</v>
       </c>
-      <c r="C3" s="90" t="s">
+      <c r="C3" s="88" t="s">
         <v>16</v>
       </c>
-      <c r="D3" s="87">
+      <c r="D3" s="85">
         <v>-95257.22</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="18.75">
-      <c r="A4" s="90" t="s">
+    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="19.5">
+      <c r="A4" s="88" t="s">
         <v>79</v>
       </c>
-      <c r="B4" s="90" t="s">
+      <c r="B4" s="88" t="s">
         <v>19</v>
       </c>
-      <c r="C4" s="90" t="s">
+      <c r="C4" s="88" t="s">
         <v>81</v>
       </c>
-      <c r="D4" s="87">
+      <c r="D4" s="85">
         <v>0</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="18.75">
-      <c r="A5" s="90" t="s">
+    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="19.5">
+      <c r="A5" s="88" t="s">
         <v>79</v>
       </c>
-      <c r="B5" s="90" t="s">
+      <c r="B5" s="88" t="s">
         <v>20</v>
       </c>
-      <c r="C5" s="90" t="s">
+      <c r="C5" s="88" t="s">
         <v>20</v>
       </c>
-      <c r="D5" s="87">
+      <c r="D5" s="85">
         <v>0</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="18.75">
-      <c r="A6" s="90" t="s">
+    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="19.5">
+      <c r="A6" s="88" t="s">
         <v>79</v>
       </c>
-      <c r="B6" s="90" t="s">
+      <c r="B6" s="88" t="s">
         <v>20</v>
       </c>
-      <c r="C6" s="90" t="s">
+      <c r="C6" s="88" t="s">
         <v>21</v>
       </c>
-      <c r="D6" s="87">
+      <c r="D6" s="85">
         <v>0</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="18.75">
-      <c r="A7" s="90" t="s">
+    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="19.5">
+      <c r="A7" s="88" t="s">
         <v>79</v>
       </c>
-      <c r="B7" s="90" t="s">
+      <c r="B7" s="88" t="s">
         <v>24</v>
       </c>
-      <c r="C7" s="90" t="s">
+      <c r="C7" s="88" t="s">
         <v>25</v>
       </c>
-      <c r="D7" s="87">
+      <c r="D7" s="85">
         <v>-285</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="18.75">
-      <c r="A8" s="90" t="s">
+    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="19.5">
+      <c r="A8" s="88" t="s">
         <v>79</v>
       </c>
-      <c r="B8" s="90" t="s">
+      <c r="B8" s="88" t="s">
         <v>24</v>
       </c>
-      <c r="C8" s="90" t="s">
+      <c r="C8" s="88" t="s">
         <v>27</v>
       </c>
-      <c r="D8" s="87">
+      <c r="D8" s="85">
         <v>0</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="18.75">
-      <c r="A9" s="90" t="s">
+    <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="19.5">
+      <c r="A9" s="88" t="s">
         <v>79</v>
       </c>
-      <c r="B9" s="90" t="s">
+      <c r="B9" s="88" t="s">
         <v>24</v>
       </c>
-      <c r="C9" s="90" t="s">
+      <c r="C9" s="88" t="s">
         <v>49</v>
       </c>
-      <c r="D9" s="87">
+      <c r="D9" s="85">
         <v>-1075407.5</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="18.75">
-      <c r="A10" s="90" t="s">
+    <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="19.5">
+      <c r="A10" s="88" t="s">
         <v>79</v>
       </c>
-      <c r="B10" s="90" t="s">
+      <c r="B10" s="88" t="s">
         <v>82</v>
       </c>
-      <c r="C10" s="90" t="s">
+      <c r="C10" s="88" t="s">
         <v>57</v>
       </c>
-      <c r="D10" s="87">
+      <c r="D10" s="85">
         <v>-8742</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="18.75">
-      <c r="A11" s="90" t="s">
+    <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="19.5">
+      <c r="A11" s="88" t="s">
         <v>79</v>
       </c>
-      <c r="B11" s="90" t="s">
+      <c r="B11" s="88" t="s">
         <v>82</v>
       </c>
-      <c r="C11" s="90" t="s">
+      <c r="C11" s="88" t="s">
         <v>58</v>
       </c>
-      <c r="D11" s="87">
+      <c r="D11" s="85">
         <v>0</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="18.75">
-      <c r="A12" s="90" t="s">
+    <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="19.5">
+      <c r="A12" s="88" t="s">
         <v>79</v>
       </c>
-      <c r="B12" s="90" t="s">
+      <c r="B12" s="88" t="s">
         <v>83</v>
       </c>
-      <c r="C12" s="90" t="s">
+      <c r="C12" s="88" t="s">
         <v>84</v>
       </c>
-      <c r="D12" s="87">
+      <c r="D12" s="85">
         <v>0</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="18.75">
-      <c r="A13" s="90" t="s">
+    <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="19.5">
+      <c r="A13" s="88" t="s">
         <v>79</v>
       </c>
-      <c r="B13" s="90" t="s">
+      <c r="B13" s="88" t="s">
         <v>83</v>
       </c>
-      <c r="C13" s="90" t="s">
+      <c r="C13" s="88" t="s">
         <v>85</v>
       </c>
-      <c r="D13" s="87">
+      <c r="D13" s="85">
         <v>0</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="18.75">
-      <c r="A14" s="90" t="s">
+    <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="19.5">
+      <c r="A14" s="88" t="s">
         <v>86</v>
       </c>
-      <c r="B14" s="90" t="s">
+      <c r="B14" s="88" t="s">
         <v>87</v>
       </c>
-      <c r="C14" s="90" t="s">
+      <c r="C14" s="88" t="s">
         <v>88</v>
       </c>
-      <c r="D14" s="91">
-        <v>32330.6</v>
+      <c r="D14" s="89">
+        <v>80826.5</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="19.5">
-      <c r="A15" s="90" t="s">
+      <c r="A15" s="88" t="s">
         <v>79</v>
       </c>
-      <c r="B15" s="90" t="s">
+      <c r="B15" s="88" t="s">
         <v>89</v>
       </c>
-      <c r="C15" s="92" t="s">
+      <c r="C15" s="90" t="s">
         <v>90</v>
       </c>
       <c r="D15" s="24">
         <v>0.05</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="16" customHeight="1" ht="19.5">
+      <c r="A16" s="88" t="s">
+        <v>79</v>
+      </c>
+      <c r="B16" s="88" t="s">
+        <v>89</v>
+      </c>
+      <c r="C16" s="90" t="s">
+        <v>91</v>
+      </c>
+      <c r="D16" s="24">
+        <v>0.15</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="17" customHeight="1" ht="19.5">
+      <c r="A17" s="88" t="s">
+        <v>89</v>
+      </c>
+      <c r="B17" s="88" t="s">
+        <v>89</v>
+      </c>
+      <c r="C17" s="90" t="s">
+        <v>92</v>
+      </c>
+      <c r="D17" s="89">
+        <v>1045</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="18" customHeight="1" ht="19.5">
+      <c r="A18" s="88" t="s">
+        <v>89</v>
+      </c>
+      <c r="B18" s="88" t="s">
+        <v>89</v>
+      </c>
+      <c r="C18" s="90" t="s">
+        <v>93</v>
+      </c>
+      <c r="D18" s="24">
+        <v>0.15</v>
       </c>
     </row>
   </sheetData>
@@ -1358,98 +1397,98 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" style="88" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="88" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="88" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="4" max="4" style="88" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="5" max="5" style="88" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="6" max="6" style="88" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="7" max="7" style="88" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="8" max="8" style="88" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="9" max="9" style="88" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="10" max="10" style="88" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="11" max="11" style="88" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="12" max="12" style="88" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="13" max="13" style="88" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" style="86" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="86" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="3" max="3" style="86" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="4" max="4" style="86" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="5" max="5" style="86" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="6" max="6" style="86" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="7" max="7" style="86" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="8" max="8" style="86" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="9" max="9" style="86" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="10" max="10" style="86" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="11" max="11" style="86" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="12" max="12" style="86" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="13" max="13" style="86" width="13.576428571428572" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
     <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="18.75">
-      <c r="A1" s="85"/>
-      <c r="B1" s="86" t="s">
+      <c r="A1" s="83"/>
+      <c r="B1" s="84" t="s">
         <v>63</v>
       </c>
-      <c r="C1" s="86" t="s">
+      <c r="C1" s="84" t="s">
         <v>64</v>
       </c>
-      <c r="D1" s="86" t="s">
+      <c r="D1" s="84" t="s">
         <v>65</v>
       </c>
-      <c r="E1" s="86" t="s">
+      <c r="E1" s="84" t="s">
         <v>66</v>
       </c>
-      <c r="F1" s="86" t="s">
+      <c r="F1" s="84" t="s">
         <v>67</v>
       </c>
-      <c r="G1" s="86" t="s">
+      <c r="G1" s="84" t="s">
         <v>68</v>
       </c>
-      <c r="H1" s="86" t="s">
+      <c r="H1" s="84" t="s">
         <v>69</v>
       </c>
-      <c r="I1" s="86" t="s">
+      <c r="I1" s="84" t="s">
         <v>70</v>
       </c>
-      <c r="J1" s="86" t="s">
+      <c r="J1" s="84" t="s">
         <v>71</v>
       </c>
-      <c r="K1" s="86" t="s">
+      <c r="K1" s="84" t="s">
         <v>72</v>
       </c>
-      <c r="L1" s="86" t="s">
+      <c r="L1" s="84" t="s">
         <v>73</v>
       </c>
-      <c r="M1" s="86" t="s">
+      <c r="M1" s="84" t="s">
         <v>74</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="18.75">
-      <c r="A2" s="87">
+      <c r="A2" s="85">
         <v>2023</v>
       </c>
-      <c r="B2" s="87">
+      <c r="B2" s="85">
         <v>85612</v>
       </c>
-      <c r="C2" s="87">
+      <c r="C2" s="85">
         <v>64741</v>
       </c>
-      <c r="D2" s="87">
+      <c r="D2" s="85">
         <v>61944</v>
       </c>
-      <c r="E2" s="87">
+      <c r="E2" s="85">
         <v>84092</v>
       </c>
-      <c r="F2" s="87">
+      <c r="F2" s="85">
         <v>70168</v>
       </c>
-      <c r="G2" s="87">
+      <c r="G2" s="85">
         <v>74058</v>
       </c>
-      <c r="H2" s="87">
+      <c r="H2" s="85">
         <v>82358</v>
       </c>
-      <c r="I2" s="87">
+      <c r="I2" s="85">
         <v>84442</v>
       </c>
-      <c r="J2" s="87">
+      <c r="J2" s="85">
         <v>70080</v>
       </c>
-      <c r="K2" s="87">
+      <c r="K2" s="85">
         <v>81539</v>
       </c>
-      <c r="L2" s="87">
+      <c r="L2" s="85">
         <v>82282</v>
       </c>
-      <c r="M2" s="87">
+      <c r="M2" s="85">
         <v>73065</v>
       </c>
     </row>
@@ -1471,27 +1510,27 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" style="77" width="31.14785714285714" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="78" width="14.719285714285713" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="79" width="6.862142857142857" customWidth="1" bestFit="1"/>
-    <col min="4" max="4" style="80" width="13.719285714285713" customWidth="1" bestFit="1"/>
-    <col min="5" max="5" style="79" width="7.433571428571429" customWidth="1" bestFit="1"/>
-    <col min="6" max="6" style="80" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="7" max="7" style="79" width="7.2907142857142855" customWidth="1" bestFit="1"/>
-    <col min="8" max="8" style="77" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="9" max="9" style="81" width="7.005" customWidth="1" bestFit="1"/>
-    <col min="10" max="10" style="78" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="11" max="11" style="82" width="7.2907142857142855" customWidth="1" bestFit="1"/>
-    <col min="12" max="12" style="80" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="13" max="13" style="82" width="7.005" customWidth="1" bestFit="1"/>
-    <col min="14" max="14" style="78" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="15" max="15" style="82" width="6.433571428571429" customWidth="1" bestFit="1"/>
-    <col min="16" max="16" style="80" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="17" max="17" style="82" width="7.005" customWidth="1" bestFit="1"/>
-    <col min="18" max="18" style="83" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="19" max="19" style="82" width="7.2907142857142855" customWidth="1" bestFit="1"/>
-    <col min="20" max="20" style="82" width="17.14785714285714" customWidth="1" bestFit="1"/>
-    <col min="21" max="21" style="84" width="31.14785714285714" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" style="76" width="31.14785714285714" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="77" width="14.719285714285713" customWidth="1" bestFit="1"/>
+    <col min="3" max="3" style="78" width="6.862142857142857" customWidth="1" bestFit="1"/>
+    <col min="4" max="4" style="77" width="13.719285714285713" customWidth="1" bestFit="1"/>
+    <col min="5" max="5" style="78" width="7.433571428571429" customWidth="1" bestFit="1"/>
+    <col min="6" max="6" style="77" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="7" max="7" style="78" width="7.2907142857142855" customWidth="1" bestFit="1"/>
+    <col min="8" max="8" style="76" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="9" max="9" style="79" width="7.005" customWidth="1" bestFit="1"/>
+    <col min="10" max="10" style="77" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="11" max="11" style="80" width="7.2907142857142855" customWidth="1" bestFit="1"/>
+    <col min="12" max="12" style="77" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="13" max="13" style="80" width="7.005" customWidth="1" bestFit="1"/>
+    <col min="14" max="14" style="77" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="15" max="15" style="80" width="6.433571428571429" customWidth="1" bestFit="1"/>
+    <col min="16" max="16" style="77" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="17" max="17" style="80" width="7.005" customWidth="1" bestFit="1"/>
+    <col min="18" max="18" style="81" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="19" max="19" style="80" width="7.2907142857142855" customWidth="1" bestFit="1"/>
+    <col min="20" max="20" style="80" width="17.14785714285714" customWidth="1" bestFit="1"/>
+    <col min="21" max="21" style="82" width="31.14785714285714" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
     <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="18.75">
@@ -3382,7 +3421,7 @@
       <c r="D42" s="8"/>
       <c r="E42" s="3"/>
       <c r="F42" s="8"/>
-      <c r="G42" s="67"/>
+      <c r="G42" s="12"/>
       <c r="H42" s="8"/>
       <c r="I42" s="6"/>
       <c r="J42" s="2"/>
@@ -3407,7 +3446,7 @@
       <c r="D43" s="8"/>
       <c r="E43" s="3"/>
       <c r="F43" s="8"/>
-      <c r="G43" s="67"/>
+      <c r="G43" s="12"/>
       <c r="H43" s="8"/>
       <c r="I43" s="6"/>
       <c r="J43" s="2"/>
@@ -3487,7 +3526,7 @@
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="45" customHeight="1" ht="18.75">
-      <c r="A45" s="68" t="s">
+      <c r="A45" s="67" t="s">
         <v>58</v>
       </c>
       <c r="B45" s="8">
@@ -3653,7 +3692,7 @@
       </c>
       <c r="E49" s="3"/>
       <c r="F49" s="8"/>
-      <c r="G49" s="67"/>
+      <c r="G49" s="12"/>
       <c r="H49" s="8"/>
       <c r="I49" s="6"/>
       <c r="J49" s="8">
@@ -3763,7 +3802,7 @@
       <c r="A52" s="1"/>
       <c r="B52" s="2"/>
       <c r="C52" s="3"/>
-      <c r="D52" s="69"/>
+      <c r="D52" s="68"/>
       <c r="E52" s="42"/>
       <c r="F52" s="5"/>
       <c r="G52" s="42"/>
@@ -3786,10 +3825,10 @@
       <c r="A53" s="1"/>
       <c r="B53" s="2"/>
       <c r="C53" s="3"/>
-      <c r="D53" s="69"/>
+      <c r="D53" s="68"/>
       <c r="E53" s="64"/>
       <c r="F53" s="5"/>
-      <c r="G53" s="70"/>
+      <c r="G53" s="69"/>
       <c r="H53" s="1"/>
       <c r="I53" s="6"/>
       <c r="J53" s="2"/>
@@ -3809,7 +3848,7 @@
       <c r="A54" s="1"/>
       <c r="B54" s="2"/>
       <c r="C54" s="3"/>
-      <c r="D54" s="69"/>
+      <c r="D54" s="68"/>
       <c r="E54" s="42"/>
       <c r="F54" s="5"/>
       <c r="G54" s="42"/>
@@ -3832,7 +3871,7 @@
       <c r="A55" s="1"/>
       <c r="B55" s="2"/>
       <c r="C55" s="3"/>
-      <c r="D55" s="69"/>
+      <c r="D55" s="68"/>
       <c r="E55" s="64"/>
       <c r="F55" s="5"/>
       <c r="G55" s="45"/>
@@ -3855,10 +3894,10 @@
       <c r="A56" s="1"/>
       <c r="B56" s="2"/>
       <c r="C56" s="3"/>
-      <c r="D56" s="69"/>
-      <c r="E56" s="67"/>
+      <c r="D56" s="68"/>
+      <c r="E56" s="12"/>
       <c r="F56" s="5"/>
-      <c r="G56" s="67"/>
+      <c r="G56" s="12"/>
       <c r="H56" s="1"/>
       <c r="I56" s="6"/>
       <c r="J56" s="2"/>
@@ -3878,7 +3917,7 @@
       <c r="A57" s="1"/>
       <c r="B57" s="2"/>
       <c r="C57" s="3"/>
-      <c r="D57" s="69"/>
+      <c r="D57" s="68"/>
       <c r="E57" s="64"/>
       <c r="F57" s="5"/>
       <c r="G57" s="42"/>
@@ -3901,7 +3940,7 @@
       <c r="A58" s="1"/>
       <c r="B58" s="2"/>
       <c r="C58" s="3"/>
-      <c r="D58" s="69"/>
+      <c r="D58" s="68"/>
       <c r="E58" s="42"/>
       <c r="F58" s="5"/>
       <c r="G58" s="42"/>
@@ -3924,7 +3963,7 @@
       <c r="A59" s="1"/>
       <c r="B59" s="2"/>
       <c r="C59" s="3"/>
-      <c r="D59" s="69"/>
+      <c r="D59" s="68"/>
       <c r="E59" s="42"/>
       <c r="F59" s="5"/>
       <c r="G59" s="42"/>
@@ -3947,7 +3986,7 @@
       <c r="A60" s="1"/>
       <c r="B60" s="2"/>
       <c r="C60" s="3"/>
-      <c r="D60" s="69"/>
+      <c r="D60" s="68"/>
       <c r="E60" s="64"/>
       <c r="F60" s="5"/>
       <c r="G60" s="42"/>
@@ -3970,7 +4009,7 @@
       <c r="A61" s="1"/>
       <c r="B61" s="2"/>
       <c r="C61" s="3"/>
-      <c r="D61" s="71"/>
+      <c r="D61" s="70"/>
       <c r="E61" s="42"/>
       <c r="F61" s="5"/>
       <c r="G61" s="42"/>
@@ -3993,10 +4032,10 @@
       <c r="A62" s="1"/>
       <c r="B62" s="2"/>
       <c r="C62" s="3"/>
-      <c r="D62" s="69"/>
+      <c r="D62" s="68"/>
       <c r="E62" s="64"/>
       <c r="F62" s="5"/>
-      <c r="G62" s="70"/>
+      <c r="G62" s="69"/>
       <c r="H62" s="1"/>
       <c r="I62" s="6"/>
       <c r="J62" s="2"/>
@@ -4016,7 +4055,7 @@
       <c r="A63" s="1"/>
       <c r="B63" s="2"/>
       <c r="C63" s="3"/>
-      <c r="D63" s="72"/>
+      <c r="D63" s="71"/>
       <c r="E63" s="42"/>
       <c r="F63" s="5"/>
       <c r="G63" s="42"/>
@@ -4039,10 +4078,10 @@
       <c r="A64" s="1"/>
       <c r="B64" s="2"/>
       <c r="C64" s="3"/>
-      <c r="D64" s="73"/>
+      <c r="D64" s="72"/>
       <c r="E64" s="64"/>
       <c r="F64" s="5"/>
-      <c r="G64" s="74"/>
+      <c r="G64" s="73"/>
       <c r="H64" s="1"/>
       <c r="I64" s="6"/>
       <c r="J64" s="2"/>
@@ -4062,7 +4101,7 @@
       <c r="A65" s="1"/>
       <c r="B65" s="2"/>
       <c r="C65" s="3"/>
-      <c r="D65" s="75"/>
+      <c r="D65" s="74"/>
       <c r="E65" s="42"/>
       <c r="F65" s="5"/>
       <c r="G65" s="45"/>
@@ -4085,7 +4124,7 @@
       <c r="A66" s="1"/>
       <c r="B66" s="2"/>
       <c r="C66" s="3"/>
-      <c r="D66" s="75"/>
+      <c r="D66" s="74"/>
       <c r="E66" s="42"/>
       <c r="F66" s="5"/>
       <c r="G66" s="42"/>
@@ -4108,7 +4147,7 @@
       <c r="A67" s="1"/>
       <c r="B67" s="2"/>
       <c r="C67" s="3"/>
-      <c r="D67" s="72"/>
+      <c r="D67" s="71"/>
       <c r="E67" s="64"/>
       <c r="F67" s="5"/>
       <c r="G67" s="45"/>
@@ -4131,10 +4170,10 @@
       <c r="A68" s="1"/>
       <c r="B68" s="2"/>
       <c r="C68" s="3"/>
-      <c r="D68" s="75"/>
-      <c r="E68" s="74"/>
+      <c r="D68" s="74"/>
+      <c r="E68" s="73"/>
       <c r="F68" s="5"/>
-      <c r="G68" s="74"/>
+      <c r="G68" s="73"/>
       <c r="H68" s="1"/>
       <c r="I68" s="6"/>
       <c r="J68" s="2"/>
@@ -4154,7 +4193,7 @@
       <c r="A69" s="1"/>
       <c r="B69" s="2"/>
       <c r="C69" s="3"/>
-      <c r="D69" s="75"/>
+      <c r="D69" s="74"/>
       <c r="E69" s="3"/>
       <c r="F69" s="5"/>
       <c r="G69" s="3"/>
@@ -4177,7 +4216,7 @@
       <c r="A70" s="1"/>
       <c r="B70" s="2"/>
       <c r="C70" s="3"/>
-      <c r="D70" s="69"/>
+      <c r="D70" s="68"/>
       <c r="E70" s="3"/>
       <c r="F70" s="5"/>
       <c r="G70" s="3"/>
@@ -4200,7 +4239,7 @@
       <c r="A71" s="1"/>
       <c r="B71" s="2"/>
       <c r="C71" s="3"/>
-      <c r="D71" s="76"/>
+      <c r="D71" s="75"/>
       <c r="E71" s="3"/>
       <c r="F71" s="5"/>
       <c r="G71" s="3"/>
@@ -4223,7 +4262,7 @@
       <c r="A72" s="1"/>
       <c r="B72" s="2"/>
       <c r="C72" s="3"/>
-      <c r="D72" s="75"/>
+      <c r="D72" s="74"/>
       <c r="E72" s="3"/>
       <c r="F72" s="5"/>
       <c r="G72" s="3"/>
@@ -4246,7 +4285,7 @@
       <c r="A73" s="1"/>
       <c r="B73" s="2"/>
       <c r="C73" s="3"/>
-      <c r="D73" s="69"/>
+      <c r="D73" s="68"/>
       <c r="E73" s="3"/>
       <c r="F73" s="5"/>
       <c r="G73" s="3"/>
@@ -4269,7 +4308,7 @@
       <c r="A74" s="1"/>
       <c r="B74" s="2"/>
       <c r="C74" s="3"/>
-      <c r="D74" s="72"/>
+      <c r="D74" s="71"/>
       <c r="E74" s="3"/>
       <c r="F74" s="5"/>
       <c r="G74" s="3"/>
@@ -4292,7 +4331,7 @@
       <c r="A75" s="1"/>
       <c r="B75" s="2"/>
       <c r="C75" s="3"/>
-      <c r="D75" s="69"/>
+      <c r="D75" s="68"/>
       <c r="E75" s="3"/>
       <c r="F75" s="5"/>
       <c r="G75" s="3"/>
@@ -4315,7 +4354,7 @@
       <c r="A76" s="1"/>
       <c r="B76" s="2"/>
       <c r="C76" s="3"/>
-      <c r="D76" s="72"/>
+      <c r="D76" s="71"/>
       <c r="E76" s="3"/>
       <c r="F76" s="5"/>
       <c r="G76" s="3"/>
@@ -4338,7 +4377,7 @@
       <c r="A77" s="1"/>
       <c r="B77" s="2"/>
       <c r="C77" s="3"/>
-      <c r="D77" s="69"/>
+      <c r="D77" s="68"/>
       <c r="E77" s="3"/>
       <c r="F77" s="5"/>
       <c r="G77" s="3"/>
@@ -4361,7 +4400,7 @@
       <c r="A78" s="1"/>
       <c r="B78" s="2"/>
       <c r="C78" s="3"/>
-      <c r="D78" s="69"/>
+      <c r="D78" s="68"/>
       <c r="E78" s="3"/>
       <c r="F78" s="5"/>
       <c r="G78" s="3"/>
@@ -4384,7 +4423,7 @@
       <c r="A79" s="1"/>
       <c r="B79" s="2"/>
       <c r="C79" s="3"/>
-      <c r="D79" s="71"/>
+      <c r="D79" s="70"/>
       <c r="E79" s="3"/>
       <c r="F79" s="5"/>
       <c r="G79" s="3"/>
@@ -4407,7 +4446,7 @@
       <c r="A80" s="1"/>
       <c r="B80" s="2"/>
       <c r="C80" s="3"/>
-      <c r="D80" s="69"/>
+      <c r="D80" s="68"/>
       <c r="E80" s="3"/>
       <c r="F80" s="5"/>
       <c r="G80" s="3"/>
@@ -4430,7 +4469,7 @@
       <c r="A81" s="1"/>
       <c r="B81" s="2"/>
       <c r="C81" s="3"/>
-      <c r="D81" s="72"/>
+      <c r="D81" s="71"/>
       <c r="E81" s="3"/>
       <c r="F81" s="5"/>
       <c r="G81" s="3"/>
@@ -4453,7 +4492,7 @@
       <c r="A82" s="1"/>
       <c r="B82" s="2"/>
       <c r="C82" s="3"/>
-      <c r="D82" s="69"/>
+      <c r="D82" s="68"/>
       <c r="E82" s="3"/>
       <c r="F82" s="5"/>
       <c r="G82" s="3"/>
@@ -4476,7 +4515,7 @@
       <c r="A83" s="1"/>
       <c r="B83" s="2"/>
       <c r="C83" s="3"/>
-      <c r="D83" s="72"/>
+      <c r="D83" s="71"/>
       <c r="E83" s="3"/>
       <c r="F83" s="5"/>
       <c r="G83" s="3"/>
@@ -4499,7 +4538,7 @@
       <c r="A84" s="1"/>
       <c r="B84" s="2"/>
       <c r="C84" s="3"/>
-      <c r="D84" s="69"/>
+      <c r="D84" s="68"/>
       <c r="E84" s="3"/>
       <c r="F84" s="5"/>
       <c r="G84" s="3"/>
@@ -4522,7 +4561,7 @@
       <c r="A85" s="1"/>
       <c r="B85" s="2"/>
       <c r="C85" s="3"/>
-      <c r="D85" s="72"/>
+      <c r="D85" s="71"/>
       <c r="E85" s="3"/>
       <c r="F85" s="5"/>
       <c r="G85" s="3"/>
@@ -4545,7 +4584,7 @@
       <c r="A86" s="1"/>
       <c r="B86" s="2"/>
       <c r="C86" s="3"/>
-      <c r="D86" s="69"/>
+      <c r="D86" s="68"/>
       <c r="E86" s="3"/>
       <c r="F86" s="5"/>
       <c r="G86" s="3"/>
@@ -4568,7 +4607,7 @@
       <c r="A87" s="1"/>
       <c r="B87" s="2"/>
       <c r="C87" s="3"/>
-      <c r="D87" s="69"/>
+      <c r="D87" s="68"/>
       <c r="E87" s="3"/>
       <c r="F87" s="5"/>
       <c r="G87" s="3"/>
@@ -4591,7 +4630,7 @@
       <c r="A88" s="1"/>
       <c r="B88" s="2"/>
       <c r="C88" s="3"/>
-      <c r="D88" s="72"/>
+      <c r="D88" s="71"/>
       <c r="E88" s="3"/>
       <c r="F88" s="5"/>
       <c r="G88" s="3"/>
@@ -4614,7 +4653,7 @@
       <c r="A89" s="1"/>
       <c r="B89" s="2"/>
       <c r="C89" s="3"/>
-      <c r="D89" s="69"/>
+      <c r="D89" s="68"/>
       <c r="E89" s="3"/>
       <c r="F89" s="5"/>
       <c r="G89" s="3"/>
@@ -4637,7 +4676,7 @@
       <c r="A90" s="1"/>
       <c r="B90" s="2"/>
       <c r="C90" s="3"/>
-      <c r="D90" s="72"/>
+      <c r="D90" s="71"/>
       <c r="E90" s="3"/>
       <c r="F90" s="5"/>
       <c r="G90" s="3"/>
@@ -4660,7 +4699,7 @@
       <c r="A91" s="1"/>
       <c r="B91" s="2"/>
       <c r="C91" s="3"/>
-      <c r="D91" s="69"/>
+      <c r="D91" s="68"/>
       <c r="E91" s="3"/>
       <c r="F91" s="5"/>
       <c r="G91" s="3"/>
@@ -4683,7 +4722,7 @@
       <c r="A92" s="1"/>
       <c r="B92" s="2"/>
       <c r="C92" s="3"/>
-      <c r="D92" s="72"/>
+      <c r="D92" s="71"/>
       <c r="E92" s="3"/>
       <c r="F92" s="5"/>
       <c r="G92" s="3"/>
@@ -4706,7 +4745,7 @@
       <c r="A93" s="1"/>
       <c r="B93" s="2"/>
       <c r="C93" s="3"/>
-      <c r="D93" s="69"/>
+      <c r="D93" s="68"/>
       <c r="E93" s="3"/>
       <c r="F93" s="5"/>
       <c r="G93" s="3"/>
@@ -4729,7 +4768,7 @@
       <c r="A94" s="1"/>
       <c r="B94" s="2"/>
       <c r="C94" s="3"/>
-      <c r="D94" s="69"/>
+      <c r="D94" s="68"/>
       <c r="E94" s="3"/>
       <c r="F94" s="5"/>
       <c r="G94" s="3"/>
@@ -4752,7 +4791,7 @@
       <c r="A95" s="1"/>
       <c r="B95" s="2"/>
       <c r="C95" s="3"/>
-      <c r="D95" s="72"/>
+      <c r="D95" s="71"/>
       <c r="E95" s="3"/>
       <c r="F95" s="5"/>
       <c r="G95" s="3"/>

</xml_diff>